<commit_message>
Ajout de la solution dans le dossier portail (sprint 1), quelque scripts SQL et divers ajouts de fichiers dans les ressources
</commit_message>
<xml_diff>
--- a/Gestion de projet/Ressources/Couleurs.xlsx
+++ b/Gestion de projet/Ressources/Couleurs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Orange</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>#083a7c</t>
+  </si>
+  <si>
+    <t>Gris léger</t>
+  </si>
+  <si>
+    <t>#e7ecf2</t>
   </si>
 </sst>
 </file>
@@ -67,7 +73,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF083A7C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7ECF2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -126,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -144,6 +156,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +169,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE7ECF2"/>
       <color rgb="FF083A7C"/>
       <color rgb="FF0097DC"/>
       <color rgb="FF005DDC"/>
@@ -432,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G6"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +462,7 @@
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -462,7 +480,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +498,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -498,7 +516,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -516,7 +534,25 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7">
+        <v>231</v>
+      </c>
+      <c r="D6" s="7">
+        <v>236</v>
+      </c>
+      <c r="E6" s="7">
+        <v>242</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="13" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modification du fichier de couleurs / logo
</commit_message>
<xml_diff>
--- a/Gestion de projet/Ressources/Couleurs.xlsx
+++ b/Gestion de projet/Ressources/Couleurs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Orange</t>
   </si>
   <si>
-    <t>Bleu</t>
-  </si>
-  <si>
-    <t>Bleu clair</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -48,9 +42,6 @@
     <t>#f9a01b</t>
   </si>
   <si>
-    <t>#0097dc</t>
-  </si>
-  <si>
     <t>#083a7c</t>
   </si>
   <si>
@@ -58,6 +49,27 @@
   </si>
   <si>
     <t>#e7ecf2</t>
+  </si>
+  <si>
+    <t>#474747</t>
+  </si>
+  <si>
+    <t>Gris foncé</t>
+  </si>
+  <si>
+    <t>#0a4696</t>
+  </si>
+  <si>
+    <t>#0d5ec9</t>
+  </si>
+  <si>
+    <t>Bleu 2</t>
+  </si>
+  <si>
+    <t>Bleu 1</t>
+  </si>
+  <si>
+    <t>Bleu 3</t>
   </si>
 </sst>
 </file>
@@ -73,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,12 +106,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0097DC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF083A7C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -107,6 +113,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7ECF2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF474747"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0D5EC9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0A4696"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -153,14 +177,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,11 +202,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFE7ECF2"/>
+      <color rgb="FF0A4696"/>
+      <color rgb="FF0D5EC9"/>
+      <color rgb="FF474747"/>
+      <color rgb="FF3D5B83"/>
+      <color rgb="FF476A99"/>
       <color rgb="FF083A7C"/>
-      <color rgb="FF0097DC"/>
-      <color rgb="FF005DDC"/>
-      <color rgb="FFF9A01B"/>
+      <color rgb="FF3557B7"/>
+      <color rgb="FF236AC9"/>
+      <color rgb="FF086BE3"/>
+      <color rgb="FF216BE3"/>
     </mruColors>
   </colors>
   <extLst>
@@ -450,37 +488,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G13"/>
+  <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,13 +532,13 @@
         <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
@@ -512,47 +550,86 @@
         <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
       <c r="D5" s="1">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>94</v>
+      </c>
+      <c r="E6" s="1">
+        <v>201</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>71</v>
+      </c>
+      <c r="D7" s="1">
+        <v>71</v>
+      </c>
+      <c r="E7" s="1">
+        <v>71</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>231</v>
+      </c>
+      <c r="D8" s="6">
+        <v>236</v>
+      </c>
+      <c r="E8" s="6">
+        <v>242</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7">
-        <v>231</v>
-      </c>
-      <c r="D6" s="7">
-        <v>236</v>
-      </c>
-      <c r="E6" s="7">
-        <v>242</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="13" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="15" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>